<commit_message>
Finalizacion de unidad 4
</commit_message>
<xml_diff>
--- a/Documentacion/INFORME FINAL/Teoria-Leida.xlsx
+++ b/Documentacion/INFORME FINAL/Teoria-Leida.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Capitulos</t>
   </si>
@@ -398,7 +398,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -443,6 +443,9 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
@@ -450,6 +453,9 @@
     <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">

</xml_diff>

<commit_message>
leido y corregido cap 2
</commit_message>
<xml_diff>
--- a/Documentacion/INFORME FINAL/Teoria-Leida.xlsx
+++ b/Documentacion/INFORME FINAL/Teoria-Leida.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Capitulos</t>
   </si>
@@ -398,7 +398,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -436,7 +436,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -456,6 +456,9 @@
       </c>
       <c r="B5" t="s">
         <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3">

</xml_diff>

<commit_message>
Refinamiento de documentacion-unidad 5 terminada
</commit_message>
<xml_diff>
--- a/Documentacion/INFORME FINAL/Teoria-Leida.xlsx
+++ b/Documentacion/INFORME FINAL/Teoria-Leida.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Capitulos</t>
   </si>
@@ -66,7 +66,7 @@
     <t>Leida</t>
   </si>
   <si>
-    <t>proceso</t>
+    <t>Preceso</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -472,12 +472,15 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3">

</xml_diff>

<commit_message>
cambios en teoria leida
</commit_message>
<xml_diff>
--- a/Documentacion/INFORME FINAL/Teoria-Leida.xlsx
+++ b/Documentacion/INFORME FINAL/Teoria-Leida.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Capitulos</t>
   </si>
@@ -60,13 +60,13 @@
     <t>3-Analisis y Evaluacion de Tecnlogias</t>
   </si>
   <si>
-    <t>En proceso</t>
-  </si>
-  <si>
     <t>Leida</t>
   </si>
   <si>
     <t>Preceso</t>
+  </si>
+  <si>
+    <t>enProceso</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -450,7 +450,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -464,7 +464,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -474,18 +474,24 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3">

</xml_diff>